<commit_message>
Add new tracker abbreviations
</commit_message>
<xml_diff>
--- a/import-specification/devices/tracker.xlsx
+++ b/import-specification/devices/tracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>Field Type</t>
   </si>
@@ -141,6 +141,27 @@
   </si>
   <si>
     <t>datapoints</t>
+  </si>
+  <si>
+    <t>ACC_X</t>
+  </si>
+  <si>
+    <t>m/s²</t>
+  </si>
+  <si>
+    <t>Sensor acceleration on east-west axis</t>
+  </si>
+  <si>
+    <t>ACC_Y</t>
+  </si>
+  <si>
+    <t>Sensor acceleration on north-south axis</t>
+  </si>
+  <si>
+    <t>ACC_Z</t>
+  </si>
+  <si>
+    <t>Sensor acceleration on vertical axis</t>
   </si>
   <si>
     <t>AZIMUTH</t>
@@ -575,7 +596,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -848,10 +869,10 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -859,13 +880,13 @@
         <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -873,13 +894,13 @@
         <v>41</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8">
@@ -887,10 +908,13 @@
         <v>41</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>56</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -898,10 +922,10 @@
         <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="D19" t="s">
         <v>59</v>
@@ -914,6 +938,9 @@
       <c r="B20" t="s">
         <v>60</v>
       </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
       <c r="D20" t="s">
         <v>61</v>
       </c>
@@ -936,8 +963,11 @@
       <c r="B22" t="s">
         <v>64</v>
       </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
       <c r="D22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8">
@@ -945,10 +975,10 @@
         <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -956,10 +986,43 @@
         <v>41</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="D26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>